<commit_message>
Fixed the bug with the delay function. Now I use timer = new System.Threading.Timer((obj) =>
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/SAVE/SAVEBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/SAVE/SAVEBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Method</t>
+  </si>
+  <si>
+    <t>Bag</t>
   </si>
 </sst>
 </file>
@@ -101,8 +104,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,13 +387,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
@@ -405,7 +409,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -446,6 +450,94 @@
       </c>
       <c r="N1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>42609.645115740743</v>
+      </c>
+      <c r="B2">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>60</v>
+      </c>
+      <c r="D2">
+        <v>38</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+      <c r="G2">
+        <v>24516</v>
+      </c>
+      <c r="H2">
+        <v>19950</v>
+      </c>
+      <c r="I2">
+        <v>2519</v>
+      </c>
+      <c r="J2">
+        <v>250</v>
+      </c>
+      <c r="K2">
+        <v>160</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>2</v>
+      </c>
+      <c r="N2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>42609.64702546296</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>58</v>
+      </c>
+      <c r="D3">
+        <v>38</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <v>8991</v>
+      </c>
+      <c r="H3">
+        <v>15219</v>
+      </c>
+      <c r="I3">
+        <v>1686</v>
+      </c>
+      <c r="J3">
+        <v>202</v>
+      </c>
+      <c r="K3">
+        <v>134</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>